<commit_message>
Add FacultyName lookup property to the Room entity for the speed improvements.
</commit_message>
<xml_diff>
--- a/RoomOccupancy.Persistence/Initializer/Files/Wydziały.xlsx
+++ b/RoomOccupancy.Persistence/Initializer/Files/Wydziały.xlsx
@@ -35,9 +35,6 @@
     <t>Wydział Technologii Drewna</t>
   </si>
   <si>
-    <t>WZIM</t>
-  </si>
-  <si>
     <t>WMW</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Nazwa skrócona</t>
+  </si>
+  <si>
+    <t>WZIiM</t>
   </si>
 </sst>
 </file>
@@ -162,7 +162,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -184,23 +184,6 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -554,7 +537,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,18 +548,18 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -584,31 +567,31 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -616,31 +599,31 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -648,31 +631,31 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>